<commit_message>
updates for better user experience
</commit_message>
<xml_diff>
--- a/Server/Search Recomendations.xlsx
+++ b/Server/Search Recomendations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\structuraWeb\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A66AF-63B2-454B-835A-7F4B375408D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9477FCDA-2308-4D5D-8BD5-B5F4ACE64413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2C755B49-6FAC-49C1-B0D3-C69B8A0D71FA}"/>
   </bookViews>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DCF00C-815A-4C09-A24A-8440464B063A}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>